<commit_message>
removed some of the variables and renamed them
</commit_message>
<xml_diff>
--- a/data/lalashan_18_spe-env.xlsx
+++ b/data/lalashan_18_spe-env.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="spe" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="133">
   <si>
     <t>Acermorr</t>
   </si>
@@ -359,18 +359,6 @@
     <t>Plot_ID</t>
   </si>
   <si>
-    <t>Elevation</t>
-  </si>
-  <si>
-    <t>Aspect_folded</t>
-  </si>
-  <si>
-    <t>Slope</t>
-  </si>
-  <si>
-    <t>Heatload</t>
-  </si>
-  <si>
     <t>MAT</t>
   </si>
   <si>
@@ -389,15 +377,9 @@
     <t>frosty_days</t>
   </si>
   <si>
-    <t>Soil_depth</t>
-  </si>
-  <si>
     <t>pH_H2O</t>
   </si>
   <si>
-    <t>pH_KCl</t>
-  </si>
-  <si>
     <t>Ca</t>
   </si>
   <si>
@@ -431,10 +413,19 @@
     <t>Total_C</t>
   </si>
   <si>
-    <t>k_decomp</t>
-  </si>
-  <si>
-    <t>S_decomp</t>
+    <t>elevation</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>heatload</t>
+  </si>
+  <si>
+    <t>folded_aspect</t>
+  </si>
+  <si>
+    <t>soil_depth</t>
   </si>
 </sst>
 </file>
@@ -491,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -505,9 +496,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,7 +778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CN19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:CN19"/>
     </sheetView>
   </sheetViews>
@@ -6083,96 +6071,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA19"/>
+  <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="N1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="O1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="P1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="T1" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>135</v>
-      </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -6213,49 +6194,40 @@
         <v>3.0470000000000002</v>
       </c>
       <c r="N2" s="6">
-        <v>2.3210000000000002</v>
+        <v>18.939810873950201</v>
       </c>
       <c r="O2" s="6">
-        <v>18.939810873950201</v>
+        <v>4.62976191219324E-2</v>
       </c>
       <c r="P2" s="6">
-        <v>4.62976191219324E-2</v>
+        <v>38.226334278370302</v>
       </c>
       <c r="Q2" s="6">
-        <v>38.226334278370302</v>
+        <v>9.6355579594415506</v>
       </c>
       <c r="R2" s="6">
-        <v>9.6355579594415506</v>
+        <v>13.8517460707798</v>
       </c>
       <c r="S2" s="6">
-        <v>13.8517460707798</v>
+        <v>0.97751136798629701</v>
       </c>
       <c r="T2" s="6">
-        <v>0.97751136798629701</v>
+        <v>4.5225641412797701</v>
       </c>
       <c r="U2" s="6">
-        <v>4.5225641412797701</v>
+        <v>0.88008405315292204</v>
       </c>
       <c r="V2" s="6">
-        <v>0.88008405315292204</v>
+        <v>19.098583774580401</v>
       </c>
       <c r="W2" s="6">
-        <v>19.098583774580401</v>
+        <v>1.4483569999999999</v>
       </c>
       <c r="X2" s="6">
-        <v>1.4483569999999999</v>
-      </c>
-      <c r="Y2" s="6">
         <v>27.6615675</v>
       </c>
-      <c r="Z2" s="6">
-        <v>1.36171981666667E-2</v>
-      </c>
-      <c r="AA2" s="6">
-        <v>0.22856721866666699</v>
-      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>92</v>
       </c>
@@ -6296,49 +6268,40 @@
         <v>2.9540000000000002</v>
       </c>
       <c r="N3" s="6">
-        <v>2.11</v>
+        <v>25.794983239271598</v>
       </c>
       <c r="O3" s="6">
-        <v>25.794983239271598</v>
+        <v>7.4005345819635901E-2</v>
       </c>
       <c r="P3" s="6">
-        <v>7.4005345819635901E-2</v>
+        <v>32.668805262511903</v>
       </c>
       <c r="Q3" s="6">
-        <v>32.668805262511903</v>
+        <v>25.415881827961201</v>
       </c>
       <c r="R3" s="6">
-        <v>25.415881827961201</v>
+        <v>34.749927428472397</v>
       </c>
       <c r="S3" s="6">
-        <v>34.749927428472397</v>
+        <v>0.69904116700170005</v>
       </c>
       <c r="T3" s="6">
-        <v>0.69904116700170005</v>
+        <v>6.41581104692622</v>
       </c>
       <c r="U3" s="6">
-        <v>6.41581104692622</v>
+        <v>2.23079115001886</v>
       </c>
       <c r="V3" s="6">
-        <v>2.23079115001886</v>
+        <v>27.7388264627685</v>
       </c>
       <c r="W3" s="6">
-        <v>27.7388264627685</v>
+        <v>1.294241</v>
       </c>
       <c r="X3" s="6">
-        <v>1.294241</v>
-      </c>
-      <c r="Y3" s="6">
         <v>35.900726499999998</v>
       </c>
-      <c r="Z3" s="6">
-        <v>1.4554754600000001E-2</v>
-      </c>
-      <c r="AA3" s="6">
-        <v>0.21432960940000001</v>
-      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>93</v>
       </c>
@@ -6379,49 +6342,40 @@
         <v>3.68</v>
       </c>
       <c r="N4" s="6">
-        <v>2.97</v>
+        <v>11.4248608146585</v>
       </c>
       <c r="O4" s="6">
-        <v>11.4248608146585</v>
+        <v>3.9778897236848999E-2</v>
       </c>
       <c r="P4" s="6">
-        <v>3.9778897236848999E-2</v>
+        <v>44.5907325939164</v>
       </c>
       <c r="Q4" s="6">
-        <v>44.5907325939164</v>
+        <v>11.2579390774233</v>
       </c>
       <c r="R4" s="6">
-        <v>11.2579390774233</v>
+        <v>8.8230937693630498</v>
       </c>
       <c r="S4" s="6">
-        <v>8.8230937693630498</v>
+        <v>2.3113979375418801</v>
       </c>
       <c r="T4" s="6">
-        <v>2.3113979375418801</v>
+        <v>1.87410674780105</v>
       </c>
       <c r="U4" s="6">
-        <v>1.87410674780105</v>
+        <v>0.31104353755542102</v>
       </c>
       <c r="V4" s="6">
-        <v>0.31104353755542102</v>
+        <v>14.6417454218531</v>
       </c>
       <c r="W4" s="6">
-        <v>14.6417454218531</v>
+        <v>0.93432999999999999</v>
       </c>
       <c r="X4" s="6">
-        <v>0.93432999999999999</v>
-      </c>
-      <c r="Y4" s="6">
         <v>13.680222000000001</v>
       </c>
-      <c r="Z4" s="6">
-        <v>1.1483294999999999E-2</v>
-      </c>
-      <c r="AA4" s="6">
-        <v>0.1067652464</v>
-      </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>94</v>
       </c>
@@ -6462,49 +6416,40 @@
         <v>3.5059999999999998</v>
       </c>
       <c r="N5" s="6">
-        <v>3.3</v>
+        <v>10.228565515894701</v>
       </c>
       <c r="O5" s="6">
-        <v>10.228565515894701</v>
+        <v>3.2345943807963601E-2</v>
       </c>
       <c r="P5" s="6">
-        <v>3.2345943807963601E-2</v>
+        <v>26.949882574614101</v>
       </c>
       <c r="Q5" s="6">
-        <v>26.949882574614101</v>
+        <v>11.169998294241999</v>
       </c>
       <c r="R5" s="6">
-        <v>11.169998294241999</v>
+        <v>6.5358745123857398</v>
       </c>
       <c r="S5" s="6">
-        <v>6.5358745123857398</v>
+        <v>1.3281045709435799</v>
       </c>
       <c r="T5" s="6">
-        <v>1.3281045709435799</v>
+        <v>2.85985170904695</v>
       </c>
       <c r="U5" s="6">
-        <v>2.85985170904695</v>
+        <v>0.33985350292187599</v>
       </c>
       <c r="V5" s="6">
-        <v>0.33985350292187599</v>
+        <v>15.785966644590999</v>
       </c>
       <c r="W5" s="6">
-        <v>15.785966644590999</v>
+        <v>1.6284915</v>
       </c>
       <c r="X5" s="6">
-        <v>1.6284915</v>
-      </c>
-      <c r="Y5" s="6">
         <v>25.7073125</v>
       </c>
-      <c r="Z5" s="6">
-        <v>1.27987862E-2</v>
-      </c>
-      <c r="AA5" s="6">
-        <v>0.1457983034</v>
-      </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>95</v>
       </c>
@@ -6545,49 +6490,40 @@
         <v>3.4180000000000001</v>
       </c>
       <c r="N6" s="6">
-        <v>2.891</v>
+        <v>15.4314263946123</v>
       </c>
       <c r="O6" s="6">
-        <v>15.4314263946123</v>
+        <v>3.4146711803529198E-2</v>
       </c>
       <c r="P6" s="6">
-        <v>3.4146711803529198E-2</v>
+        <v>34.858057843551698</v>
       </c>
       <c r="Q6" s="6">
-        <v>34.858057843551698</v>
+        <v>14.490881088837799</v>
       </c>
       <c r="R6" s="6">
-        <v>14.490881088837799</v>
+        <v>9.2482468001127796</v>
       </c>
       <c r="S6" s="6">
-        <v>9.2482468001127796</v>
+        <v>1.2977686593651101</v>
       </c>
       <c r="T6" s="6">
-        <v>1.2977686593651101</v>
+        <v>4.3765418342962601</v>
       </c>
       <c r="U6" s="6">
-        <v>4.3765418342962601</v>
+        <v>0.83199038230143296</v>
       </c>
       <c r="V6" s="6">
-        <v>0.83199038230143296</v>
+        <v>15.392849340909899</v>
       </c>
       <c r="W6" s="6">
-        <v>15.392849340909899</v>
+        <v>1.9454849999999999</v>
       </c>
       <c r="X6" s="6">
-        <v>1.9454849999999999</v>
-      </c>
-      <c r="Y6" s="6">
         <v>29.946557500000001</v>
       </c>
-      <c r="Z6" s="6">
-        <v>1.5528022000000001E-2</v>
-      </c>
-      <c r="AA6" s="6">
-        <v>0.13179925679999999</v>
-      </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>96</v>
       </c>
@@ -6628,49 +6564,40 @@
         <v>3.9020000000000001</v>
       </c>
       <c r="N7" s="6">
-        <v>3.552</v>
+        <v>40.516339058225299</v>
       </c>
       <c r="O7" s="6">
-        <v>40.516339058225299</v>
+        <v>7.2301790310405706E-2</v>
       </c>
       <c r="P7" s="6">
-        <v>7.2301790310405706E-2</v>
+        <v>16.9154914983819</v>
       </c>
       <c r="Q7" s="6">
-        <v>16.9154914983819</v>
+        <v>12.4485345301433</v>
       </c>
       <c r="R7" s="6">
-        <v>12.4485345301433</v>
+        <v>7.2677376957122402</v>
       </c>
       <c r="S7" s="6">
-        <v>7.2677376957122402</v>
+        <v>7.1774996774446196</v>
       </c>
       <c r="T7" s="6">
-        <v>7.1774996774446196</v>
+        <v>3.13022821769388</v>
       </c>
       <c r="U7" s="6">
-        <v>3.13022821769388</v>
+        <v>0.32847368401358901</v>
       </c>
       <c r="V7" s="6">
-        <v>0.32847368401358901</v>
+        <v>12.501842386327301</v>
       </c>
       <c r="W7" s="6">
-        <v>12.501842386327301</v>
+        <v>1.1755135000000001</v>
       </c>
       <c r="X7" s="6">
-        <v>1.1755135000000001</v>
-      </c>
-      <c r="Y7" s="6">
         <v>14.6960845</v>
       </c>
-      <c r="Z7" s="6">
-        <v>1.6479982666666702E-2</v>
-      </c>
-      <c r="AA7" s="6">
-        <v>0.155522777333333</v>
-      </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>97</v>
       </c>
@@ -6711,49 +6638,40 @@
         <v>3.6269999999999998</v>
       </c>
       <c r="N8" s="6">
-        <v>3.0219999999999998</v>
+        <v>59.557513163232599</v>
       </c>
       <c r="O8" s="6">
-        <v>59.557513163232599</v>
+        <v>3.2727728428586199E-2</v>
       </c>
       <c r="P8" s="6">
-        <v>3.2727728428586199E-2</v>
+        <v>35.437034552062997</v>
       </c>
       <c r="Q8" s="6">
-        <v>35.437034552062997</v>
+        <v>16.746581832331898</v>
       </c>
       <c r="R8" s="6">
-        <v>16.746581832331898</v>
+        <v>8.5452479540203097</v>
       </c>
       <c r="S8" s="6">
-        <v>8.5452479540203097</v>
+        <v>2.0541757028468002</v>
       </c>
       <c r="T8" s="6">
-        <v>2.0541757028468002</v>
+        <v>2.6019260730085998</v>
       </c>
       <c r="U8" s="6">
-        <v>2.6019260730085998</v>
+        <v>0.51439292498537303</v>
       </c>
       <c r="V8" s="6">
-        <v>0.51439292498537303</v>
+        <v>14.444231499599599</v>
       </c>
       <c r="W8" s="6">
-        <v>14.444231499599599</v>
+        <v>0.96895200000000004</v>
       </c>
       <c r="X8" s="6">
-        <v>0.96895200000000004</v>
-      </c>
-      <c r="Y8" s="6">
         <v>13.995767000000001</v>
       </c>
-      <c r="Z8" s="6">
-        <v>1.47623871666667E-2</v>
-      </c>
-      <c r="AA8" s="6">
-        <v>0.17567447250000001</v>
-      </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>98</v>
       </c>
@@ -6794,49 +6712,40 @@
         <v>3.5049999999999999</v>
       </c>
       <c r="N9" s="6">
-        <v>2.6240000000000001</v>
+        <v>16.510405516382399</v>
       </c>
       <c r="O9" s="6">
-        <v>16.510405516382399</v>
+        <v>2.7433743457029001E-2</v>
       </c>
       <c r="P9" s="6">
-        <v>2.7433743457029001E-2</v>
+        <v>39.903306611932898</v>
       </c>
       <c r="Q9" s="6">
-        <v>39.903306611932898</v>
+        <v>8.0710098367731309</v>
       </c>
       <c r="R9" s="6">
-        <v>8.0710098367731309</v>
+        <v>8.2868857824889304</v>
       </c>
       <c r="S9" s="6">
-        <v>8.2868857824889304</v>
+        <v>0.23158191012667501</v>
       </c>
       <c r="T9" s="6">
-        <v>0.23158191012667501</v>
+        <v>1.24402573848996</v>
       </c>
       <c r="U9" s="6">
-        <v>1.24402573848996</v>
+        <v>0.55674785900834001</v>
       </c>
       <c r="V9" s="6">
-        <v>0.55674785900834001</v>
+        <v>20.662495083262801</v>
       </c>
       <c r="W9" s="6">
-        <v>20.662495083262801</v>
+        <v>0.36524899999999999</v>
       </c>
       <c r="X9" s="6">
-        <v>0.36524899999999999</v>
-      </c>
-      <c r="Y9" s="6">
         <v>7.5469556666666699</v>
       </c>
-      <c r="Z9" s="6">
-        <v>1.2156222750000001E-2</v>
-      </c>
-      <c r="AA9" s="6">
-        <v>0.18454762375</v>
-      </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>99</v>
       </c>
@@ -6877,49 +6786,40 @@
         <v>3.4510000000000001</v>
       </c>
       <c r="N10" s="6">
-        <v>2.7570000000000001</v>
+        <v>54.310719788011603</v>
       </c>
       <c r="O10" s="6">
-        <v>54.310719788011603</v>
+        <v>0.104845785630615</v>
       </c>
       <c r="P10" s="6">
-        <v>0.104845785630615</v>
+        <v>32.511771087935998</v>
       </c>
       <c r="Q10" s="6">
-        <v>32.511771087935998</v>
+        <v>26.6395349460266</v>
       </c>
       <c r="R10" s="6">
-        <v>26.6395349460266</v>
+        <v>28.297227714771601</v>
       </c>
       <c r="S10" s="6">
-        <v>28.297227714771601</v>
+        <v>4.6346349134705704</v>
       </c>
       <c r="T10" s="6">
-        <v>4.6346349134705704</v>
+        <v>10.2538137128233</v>
       </c>
       <c r="U10" s="6">
-        <v>10.2538137128233</v>
+        <v>1.3261183403497201</v>
       </c>
       <c r="V10" s="6">
-        <v>1.3261183403497201</v>
+        <v>18.081914061132501</v>
       </c>
       <c r="W10" s="6">
-        <v>18.081914061132501</v>
+        <v>1.8995945000000001</v>
       </c>
       <c r="X10" s="6">
-        <v>1.8995945000000001</v>
-      </c>
-      <c r="Y10" s="6">
         <v>34.348304499999998</v>
       </c>
-      <c r="Z10" s="6">
-        <v>1.8483550800000002E-2</v>
-      </c>
-      <c r="AA10" s="6">
-        <v>0.1579814044</v>
-      </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>100</v>
       </c>
@@ -6960,49 +6860,40 @@
         <v>3.52</v>
       </c>
       <c r="N11" s="6">
-        <v>3.1880000000000002</v>
+        <v>7.8873748355647004</v>
       </c>
       <c r="O11" s="6">
-        <v>7.8873748355647004</v>
+        <v>4.7716733687252301E-2</v>
       </c>
       <c r="P11" s="6">
-        <v>4.7716733687252301E-2</v>
+        <v>22.878180922125399</v>
       </c>
       <c r="Q11" s="6">
-        <v>22.878180922125399</v>
+        <v>11.1951537547623</v>
       </c>
       <c r="R11" s="6">
-        <v>11.1951537547623</v>
+        <v>4.2394856079559204</v>
       </c>
       <c r="S11" s="6">
-        <v>4.2394856079559204</v>
+        <v>3.1126630096009702</v>
       </c>
       <c r="T11" s="6">
-        <v>3.1126630096009702</v>
+        <v>1.0757841369232599</v>
       </c>
       <c r="U11" s="6">
-        <v>1.0757841369232599</v>
+        <v>0.205411682638415</v>
       </c>
       <c r="V11" s="6">
-        <v>0.205411682638415</v>
+        <v>15.1175137228061</v>
       </c>
       <c r="W11" s="6">
-        <v>15.1175137228061</v>
+        <v>0.91608449999999997</v>
       </c>
       <c r="X11" s="6">
-        <v>0.91608449999999997</v>
-      </c>
-      <c r="Y11" s="6">
         <v>13.84892</v>
       </c>
-      <c r="Z11" s="6">
-        <v>2.3534671333333299E-2</v>
-      </c>
-      <c r="AA11" s="6">
-        <v>0.21241800399999999</v>
-      </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>101</v>
       </c>
@@ -7043,49 +6934,40 @@
         <v>3.1509999999999998</v>
       </c>
       <c r="N12" s="6">
-        <v>2.3519999999999999</v>
+        <v>7.0330010623762904</v>
       </c>
       <c r="O12" s="6">
-        <v>7.0330010623762904</v>
+        <v>1.92639724658554E-2</v>
       </c>
       <c r="P12" s="6">
-        <v>1.92639724658554E-2</v>
+        <v>33.677604243110999</v>
       </c>
       <c r="Q12" s="6">
-        <v>33.677604243110999</v>
+        <v>7.3390278303369598</v>
       </c>
       <c r="R12" s="6">
-        <v>7.3390278303369598</v>
+        <v>12.271186948557</v>
       </c>
       <c r="S12" s="6">
-        <v>12.271186948557</v>
+        <v>0.68597338995866997</v>
       </c>
       <c r="T12" s="6">
-        <v>0.68597338995866997</v>
+        <v>1.69049521176596</v>
       </c>
       <c r="U12" s="6">
-        <v>1.69049521176596</v>
+        <v>0.56123946343326903</v>
       </c>
       <c r="V12" s="6">
-        <v>0.56123946343326903</v>
+        <v>33.932250855804902</v>
       </c>
       <c r="W12" s="6">
-        <v>33.932250855804902</v>
+        <v>0.56204399999999999</v>
       </c>
       <c r="X12" s="6">
-        <v>0.56204399999999999</v>
-      </c>
-      <c r="Y12" s="6">
         <v>19.071418000000001</v>
       </c>
-      <c r="Z12" s="6">
-        <v>1.3235436E-2</v>
-      </c>
-      <c r="AA12" s="6">
-        <v>0.14263623724999999</v>
-      </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>102</v>
       </c>
@@ -7126,49 +7008,40 @@
         <v>3.629</v>
       </c>
       <c r="N13" s="6">
-        <v>3.3130000000000002</v>
+        <v>11.5444067339904</v>
       </c>
       <c r="O13" s="6">
-        <v>11.5444067339904</v>
+        <v>8.2272502727698801E-2</v>
       </c>
       <c r="P13" s="6">
-        <v>8.2272502727698801E-2</v>
+        <v>20.184363816977299</v>
       </c>
       <c r="Q13" s="6">
-        <v>20.184363816977299</v>
+        <v>9.9681671697868808</v>
       </c>
       <c r="R13" s="6">
-        <v>9.9681671697868808</v>
+        <v>4.5074453191284096</v>
       </c>
       <c r="S13" s="6">
-        <v>4.5074453191284096</v>
+        <v>5.3081505133426203</v>
       </c>
       <c r="T13" s="6">
-        <v>5.3081505133426203</v>
+        <v>1.00528265578318</v>
       </c>
       <c r="U13" s="6">
-        <v>1.00528265578318</v>
+        <v>0.32613640900537599</v>
       </c>
       <c r="V13" s="6">
-        <v>0.32613640900537599</v>
+        <v>13.9590283961611</v>
       </c>
       <c r="W13" s="6">
-        <v>13.9590283961611</v>
+        <v>0.85909500000000005</v>
       </c>
       <c r="X13" s="6">
-        <v>0.85909500000000005</v>
-      </c>
-      <c r="Y13" s="6">
         <v>11.992131499999999</v>
       </c>
-      <c r="Z13" s="6">
-        <v>2.7351985749999998E-2</v>
-      </c>
-      <c r="AA13" s="6">
-        <v>0.18978554375000001</v>
-      </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>103</v>
       </c>
@@ -7209,49 +7082,40 @@
         <v>3.7280000000000002</v>
       </c>
       <c r="N14" s="6">
-        <v>3.3290000000000002</v>
+        <v>11.7302317979557</v>
       </c>
       <c r="O14" s="6">
-        <v>11.7302317979557</v>
+        <v>7.4875163193961994E-2</v>
       </c>
       <c r="P14" s="6">
-        <v>7.4875163193961994E-2</v>
+        <v>24.767522438697</v>
       </c>
       <c r="Q14" s="6">
-        <v>24.767522438697</v>
+        <v>13.6212552401616</v>
       </c>
       <c r="R14" s="6">
-        <v>13.6212552401616</v>
+        <v>4.4750480626728004</v>
       </c>
       <c r="S14" s="6">
-        <v>4.4750480626728004</v>
+        <v>1.1371364386041101</v>
       </c>
       <c r="T14" s="6">
-        <v>1.1371364386041101</v>
+        <v>1.06225657971508</v>
       </c>
       <c r="U14" s="6">
-        <v>1.06225657971508</v>
+        <v>0.24117379217163801</v>
       </c>
       <c r="V14" s="6">
-        <v>0.24117379217163801</v>
+        <v>14.452246797041299</v>
       </c>
       <c r="W14" s="6">
-        <v>14.452246797041299</v>
+        <v>0.98393399999999998</v>
       </c>
       <c r="X14" s="6">
-        <v>0.98393399999999998</v>
-      </c>
-      <c r="Y14" s="6">
         <v>14.220057000000001</v>
       </c>
-      <c r="Z14" s="6">
-        <v>1.4563284500000001E-2</v>
-      </c>
-      <c r="AA14" s="6">
-        <v>0.16376746950000001</v>
-      </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>104</v>
       </c>
@@ -7292,49 +7156,40 @@
         <v>3.7440000000000002</v>
       </c>
       <c r="N15" s="6">
-        <v>3.2080000000000002</v>
+        <v>10.0697683721276</v>
       </c>
       <c r="O15" s="6">
-        <v>10.0697683721276</v>
+        <v>6.3425087366589694E-2</v>
       </c>
       <c r="P15" s="6">
-        <v>6.3425087366589694E-2</v>
+        <v>26.798816988847999</v>
       </c>
       <c r="Q15" s="6">
-        <v>26.798816988847999</v>
+        <v>14.3175797731837</v>
       </c>
       <c r="R15" s="6">
-        <v>14.3175797731837</v>
+        <v>5.34815297077746</v>
       </c>
       <c r="S15" s="6">
-        <v>5.34815297077746</v>
+        <v>1.0586694857463199</v>
       </c>
       <c r="T15" s="6">
-        <v>1.0586694857463199</v>
+        <v>0.813455967938854</v>
       </c>
       <c r="U15" s="6">
-        <v>0.813455967938854</v>
+        <v>0.37035028195828501</v>
       </c>
       <c r="V15" s="6">
-        <v>0.37035028195828501</v>
+        <v>15.0845177906158</v>
       </c>
       <c r="W15" s="6">
-        <v>15.0845177906158</v>
+        <v>1.0260324999999999</v>
       </c>
       <c r="X15" s="6">
-        <v>1.0260324999999999</v>
-      </c>
-      <c r="Y15" s="6">
         <v>15.4772055</v>
       </c>
-      <c r="Z15" s="6">
-        <v>1.6952645799999999E-2</v>
-      </c>
-      <c r="AA15" s="6">
-        <v>0.1597240228</v>
-      </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>105</v>
       </c>
@@ -7375,49 +7230,40 @@
         <v>3.758</v>
       </c>
       <c r="N16" s="6">
-        <v>3.2029999999999998</v>
+        <v>8.0950004725418303</v>
       </c>
       <c r="O16" s="6">
-        <v>8.0950004725418303</v>
+        <v>5.26072308616954E-2</v>
       </c>
       <c r="P16" s="6">
-        <v>5.26072308616954E-2</v>
+        <v>32.956620001543698</v>
       </c>
       <c r="Q16" s="6">
-        <v>32.956620001543698</v>
+        <v>14.5281986351171</v>
       </c>
       <c r="R16" s="6">
-        <v>14.5281986351171</v>
+        <v>4.4128310452502504</v>
       </c>
       <c r="S16" s="6">
-        <v>4.4128310452502504</v>
+        <v>0.35397887770195002</v>
       </c>
       <c r="T16" s="6">
-        <v>0.35397887770195002</v>
+        <v>0.54577509897230603</v>
       </c>
       <c r="U16" s="6">
-        <v>0.54577509897230603</v>
+        <v>0.20666426528061399</v>
       </c>
       <c r="V16" s="6">
-        <v>0.20666426528061399</v>
+        <v>15.2735349047305</v>
       </c>
       <c r="W16" s="6">
-        <v>15.2735349047305</v>
+        <v>0.83904100000000004</v>
       </c>
       <c r="X16" s="6">
-        <v>0.83904100000000004</v>
-      </c>
-      <c r="Y16" s="6">
         <v>12.815122000000001</v>
       </c>
-      <c r="Z16" s="6">
-        <v>1.4556293999999999E-2</v>
-      </c>
-      <c r="AA16" s="6">
-        <v>0.1646907702</v>
-      </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>106</v>
       </c>
@@ -7458,49 +7304,40 @@
         <v>3.8159999999999998</v>
       </c>
       <c r="N17" s="6">
-        <v>3.3540000000000001</v>
+        <v>13.6656798217541</v>
       </c>
       <c r="O17" s="6">
-        <v>13.6656798217541</v>
+        <v>8.0558915961174801E-2</v>
       </c>
       <c r="P17" s="6">
-        <v>8.0558915961174801E-2</v>
+        <v>24.687717314978599</v>
       </c>
       <c r="Q17" s="6">
-        <v>24.687717314978599</v>
+        <v>11.9602463227596</v>
       </c>
       <c r="R17" s="6">
-        <v>11.9602463227596</v>
+        <v>5.9490683093856704</v>
       </c>
       <c r="S17" s="6">
-        <v>5.9490683093856704</v>
+        <v>3.3479205531613898</v>
       </c>
       <c r="T17" s="6">
-        <v>3.3479205531613898</v>
+        <v>0.85722566497947505</v>
       </c>
       <c r="U17" s="6">
-        <v>0.85722566497947505</v>
+        <v>0.22388578180177601</v>
       </c>
       <c r="V17" s="6">
-        <v>0.22388578180177601</v>
+        <v>13.640948442708099</v>
       </c>
       <c r="W17" s="6">
-        <v>13.640948442708099</v>
+        <v>0.61098050000000004</v>
       </c>
       <c r="X17" s="6">
-        <v>0.61098050000000004</v>
-      </c>
-      <c r="Y17" s="6">
         <v>8.3343535000000006</v>
       </c>
-      <c r="Z17" s="6">
-        <v>2.0374076200000001E-2</v>
-      </c>
-      <c r="AA17" s="6">
-        <v>0.18212515100000001</v>
-      </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>107</v>
       </c>
@@ -7541,49 +7378,40 @@
         <v>3.8210000000000002</v>
       </c>
       <c r="N18" s="6">
-        <v>3.2360000000000002</v>
+        <v>7.53657865126854</v>
       </c>
       <c r="O18" s="6">
-        <v>7.53657865126854</v>
+        <v>6.8793587737153702E-2</v>
       </c>
       <c r="P18" s="6">
-        <v>6.8793587737153702E-2</v>
+        <v>31.9599542603139</v>
       </c>
       <c r="Q18" s="6">
-        <v>31.9599542603139</v>
+        <v>10.157550723003199</v>
       </c>
       <c r="R18" s="6">
-        <v>10.157550723003199</v>
+        <v>4.6777231691212702</v>
       </c>
       <c r="S18" s="6">
-        <v>4.6777231691212702</v>
+        <v>1.12728558320941</v>
       </c>
       <c r="T18" s="6">
-        <v>1.12728558320941</v>
+        <v>0.64908690361489896</v>
       </c>
       <c r="U18" s="6">
-        <v>0.64908690361489896</v>
+        <v>0.18758937220090299</v>
       </c>
       <c r="V18" s="6">
-        <v>0.18758937220090299</v>
+        <v>13.1799666378983</v>
       </c>
       <c r="W18" s="6">
-        <v>13.1799666378983</v>
+        <v>0.57760149999999999</v>
       </c>
       <c r="X18" s="6">
-        <v>0.57760149999999999</v>
-      </c>
-      <c r="Y18" s="6">
         <v>7.6127684999999996</v>
       </c>
-      <c r="Z18" s="6">
-        <v>1.8247199499999998E-2</v>
-      </c>
-      <c r="AA18" s="6">
-        <v>0.17020546349999999</v>
-      </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>108</v>
       </c>
@@ -7624,46 +7452,37 @@
         <v>3.657</v>
       </c>
       <c r="N19" s="6">
-        <v>3.1960000000000002</v>
+        <v>5.2589920423832304</v>
       </c>
       <c r="O19" s="6">
-        <v>5.2589920423832304</v>
+        <v>9.5268033294682794E-2</v>
       </c>
       <c r="P19" s="6">
-        <v>9.5268033294682794E-2</v>
+        <v>31.023532681028598</v>
       </c>
       <c r="Q19" s="6">
-        <v>31.023532681028598</v>
+        <v>10.396982831155</v>
       </c>
       <c r="R19" s="6">
-        <v>10.396982831155</v>
+        <v>5.1721543669344001</v>
       </c>
       <c r="S19" s="6">
-        <v>5.1721543669344001</v>
+        <v>1.5470265526826199</v>
       </c>
       <c r="T19" s="6">
-        <v>1.5470265526826199</v>
+        <v>0.89453986103757199</v>
       </c>
       <c r="U19" s="6">
-        <v>0.89453986103757199</v>
+        <v>0.278298814869188</v>
       </c>
       <c r="V19" s="6">
-        <v>0.278298814869188</v>
+        <v>13.548438916884599</v>
       </c>
       <c r="W19" s="6">
-        <v>13.548438916884599</v>
+        <v>0.70467100000000005</v>
       </c>
       <c r="X19" s="6">
-        <v>0.70467100000000005</v>
-      </c>
-      <c r="Y19" s="6">
         <v>9.5471920000000008</v>
-      </c>
-      <c r="Z19" s="6">
-        <v>1.9227116400000001E-2</v>
-      </c>
-      <c r="AA19" s="6">
-        <v>0.137251439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleted even by more variables
</commit_message>
<xml_diff>
--- a/data/lalashan_18_spe-env.xlsx
+++ b/data/lalashan_18_spe-env.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="spe" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="125">
   <si>
     <t>Acermorr</t>
   </si>
@@ -365,12 +365,6 @@
     <t>mean_coldest</t>
   </si>
   <si>
-    <t>mean_warmest</t>
-  </si>
-  <si>
-    <t>wet_events</t>
-  </si>
-  <si>
     <t>dry_events</t>
   </si>
   <si>
@@ -383,12 +377,6 @@
     <t>Ca</t>
   </si>
   <si>
-    <t>Cu</t>
-  </si>
-  <si>
-    <t>Fe</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -401,18 +389,9 @@
     <t>P</t>
   </si>
   <si>
-    <t>Zn</t>
-  </si>
-  <si>
     <t>CN_ratio</t>
   </si>
   <si>
-    <t>Total_N</t>
-  </si>
-  <si>
-    <t>Total_C</t>
-  </si>
-  <si>
     <t>elevation</t>
   </si>
   <si>
@@ -420,9 +399,6 @@
   </si>
   <si>
     <t>heatload</t>
-  </si>
-  <si>
-    <t>folded_aspect</t>
   </si>
   <si>
     <t>soil_depth</t>
@@ -778,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CN19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:CN19"/>
     </sheetView>
   </sheetViews>
@@ -6071,89 +6047,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X19"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>130</v>
+        <v>123</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="I1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>115</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="R1" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>127</v>
-      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -6161,73 +6113,49 @@
         <v>2082</v>
       </c>
       <c r="C2" s="4">
-        <v>135</v>
+        <v>14</v>
       </c>
       <c r="D2" s="4">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4">
         <v>1.0866453</v>
       </c>
+      <c r="E2" s="5">
+        <v>12.625595224494401</v>
+      </c>
       <c r="F2" s="5">
-        <v>12.625595224494401</v>
+        <v>7.4450127688172003</v>
       </c>
       <c r="G2" s="5">
-        <v>7.4450127688172003</v>
+        <v>4.3279569892473099E-2</v>
       </c>
       <c r="H2" s="5">
-        <v>17.125129032258101</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0.48128520225294402</v>
-      </c>
-      <c r="J2" s="5">
-        <v>4.3279569892473099E-2</v>
-      </c>
-      <c r="K2" s="5">
         <v>5</v>
       </c>
+      <c r="I2" s="6">
+        <v>28.75</v>
+      </c>
+      <c r="J2" s="6">
+        <v>3.0470000000000002</v>
+      </c>
+      <c r="K2" s="6">
+        <v>18.939810873950201</v>
+      </c>
       <c r="L2" s="6">
-        <v>28.75</v>
+        <v>9.6355579594415506</v>
       </c>
       <c r="M2" s="6">
-        <v>3.0470000000000002</v>
+        <v>13.8517460707798</v>
       </c>
       <c r="N2" s="6">
-        <v>18.939810873950201</v>
+        <v>0.97751136798629701</v>
       </c>
       <c r="O2" s="6">
-        <v>4.62976191219324E-2</v>
+        <v>4.5225641412797701</v>
       </c>
       <c r="P2" s="6">
-        <v>38.226334278370302</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>9.6355579594415506</v>
-      </c>
-      <c r="R2" s="6">
-        <v>13.8517460707798</v>
-      </c>
-      <c r="S2" s="6">
-        <v>0.97751136798629701</v>
-      </c>
-      <c r="T2" s="6">
-        <v>4.5225641412797701</v>
-      </c>
-      <c r="U2" s="6">
-        <v>0.88008405315292204</v>
-      </c>
-      <c r="V2" s="6">
         <v>19.098583774580401</v>
       </c>
-      <c r="W2" s="6">
-        <v>1.4483569999999999</v>
-      </c>
-      <c r="X2" s="6">
-        <v>27.6615675</v>
-      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>92</v>
       </c>
@@ -6235,73 +6163,49 @@
         <v>2060</v>
       </c>
       <c r="C3" s="4">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="D3" s="4">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4">
         <v>1.0782293999999999</v>
       </c>
+      <c r="E3" s="5">
+        <v>12.4214885412666</v>
+      </c>
       <c r="F3" s="5">
-        <v>12.4214885412666</v>
+        <v>7.19401612903226</v>
       </c>
       <c r="G3" s="5">
-        <v>7.19401612903226</v>
+        <v>5.4211469534050198E-2</v>
       </c>
       <c r="H3" s="5">
-        <v>16.971735887096798</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0.51418970814132103</v>
-      </c>
-      <c r="J3" s="5">
-        <v>5.4211469534050198E-2</v>
-      </c>
-      <c r="K3" s="5">
         <v>6</v>
       </c>
+      <c r="I3" s="6">
+        <v>28.660160000000001</v>
+      </c>
+      <c r="J3" s="6">
+        <v>2.9540000000000002</v>
+      </c>
+      <c r="K3" s="6">
+        <v>25.794983239271598</v>
+      </c>
       <c r="L3" s="6">
-        <v>28.660160000000001</v>
+        <v>25.415881827961201</v>
       </c>
       <c r="M3" s="6">
-        <v>2.9540000000000002</v>
+        <v>34.749927428472397</v>
       </c>
       <c r="N3" s="6">
-        <v>25.794983239271598</v>
+        <v>0.69904116700170005</v>
       </c>
       <c r="O3" s="6">
-        <v>7.4005345819635901E-2</v>
+        <v>6.41581104692622</v>
       </c>
       <c r="P3" s="6">
-        <v>32.668805262511903</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>25.415881827961201</v>
-      </c>
-      <c r="R3" s="6">
-        <v>34.749927428472397</v>
-      </c>
-      <c r="S3" s="6">
-        <v>0.69904116700170005</v>
-      </c>
-      <c r="T3" s="6">
-        <v>6.41581104692622</v>
-      </c>
-      <c r="U3" s="6">
-        <v>2.23079115001886</v>
-      </c>
-      <c r="V3" s="6">
         <v>27.7388264627685</v>
       </c>
-      <c r="W3" s="6">
-        <v>1.294241</v>
-      </c>
-      <c r="X3" s="6">
-        <v>35.900726499999998</v>
-      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>93</v>
       </c>
@@ -6309,73 +6213,49 @@
         <v>2176</v>
       </c>
       <c r="C4" s="4">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D4" s="4">
-        <v>31</v>
-      </c>
-      <c r="E4" s="4">
         <v>0.58610139999999999</v>
       </c>
+      <c r="E4" s="5">
+        <v>12.191764720666299</v>
+      </c>
       <c r="F4" s="5">
-        <v>12.191764720666299</v>
+        <v>6.7012118055555598</v>
       </c>
       <c r="G4" s="5">
-        <v>6.7012118055555598</v>
+        <v>6.6666666666666697E-3</v>
       </c>
       <c r="H4" s="5">
-        <v>16.896639784946199</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0.66708909370199698</v>
-      </c>
-      <c r="J4" s="5">
-        <v>6.6666666666666697E-3</v>
-      </c>
-      <c r="K4" s="5">
         <v>13</v>
       </c>
+      <c r="I4" s="6">
+        <v>22.847660000000001</v>
+      </c>
+      <c r="J4" s="6">
+        <v>3.68</v>
+      </c>
+      <c r="K4" s="6">
+        <v>11.4248608146585</v>
+      </c>
       <c r="L4" s="6">
-        <v>22.847660000000001</v>
+        <v>11.2579390774233</v>
       </c>
       <c r="M4" s="6">
-        <v>3.68</v>
+        <v>8.8230937693630498</v>
       </c>
       <c r="N4" s="6">
-        <v>11.4248608146585</v>
+        <v>2.3113979375418801</v>
       </c>
       <c r="O4" s="6">
-        <v>3.9778897236848999E-2</v>
+        <v>1.87410674780105</v>
       </c>
       <c r="P4" s="6">
-        <v>44.5907325939164</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>11.2579390774233</v>
-      </c>
-      <c r="R4" s="6">
-        <v>8.8230937693630498</v>
-      </c>
-      <c r="S4" s="6">
-        <v>2.3113979375418801</v>
-      </c>
-      <c r="T4" s="6">
-        <v>1.87410674780105</v>
-      </c>
-      <c r="U4" s="6">
-        <v>0.31104353755542102</v>
-      </c>
-      <c r="V4" s="6">
         <v>14.6417454218531</v>
       </c>
-      <c r="W4" s="6">
-        <v>0.93432999999999999</v>
-      </c>
-      <c r="X4" s="6">
-        <v>13.680222000000001</v>
-      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>94</v>
       </c>
@@ -6383,73 +6263,49 @@
         <v>1870</v>
       </c>
       <c r="C5" s="4">
-        <v>155</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4">
-        <v>25</v>
-      </c>
-      <c r="E5" s="4">
         <v>1.1099097</v>
       </c>
+      <c r="E5" s="5">
+        <v>13.4381557989045</v>
+      </c>
       <c r="F5" s="5">
-        <v>13.4381557989045</v>
+        <v>8.0146518817204306</v>
       </c>
       <c r="G5" s="5">
-        <v>8.0146518817204306</v>
+        <v>5.98566308243728E-2</v>
       </c>
       <c r="H5" s="5">
-        <v>18.154360215053799</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0.51848438300051203</v>
-      </c>
-      <c r="J5" s="5">
-        <v>5.98566308243728E-2</v>
-      </c>
-      <c r="K5" s="5">
         <v>6</v>
       </c>
+      <c r="I5" s="6">
+        <v>24.625</v>
+      </c>
+      <c r="J5" s="6">
+        <v>3.5059999999999998</v>
+      </c>
+      <c r="K5" s="6">
+        <v>10.228565515894701</v>
+      </c>
       <c r="L5" s="6">
-        <v>24.625</v>
+        <v>11.169998294241999</v>
       </c>
       <c r="M5" s="6">
-        <v>3.5059999999999998</v>
+        <v>6.5358745123857398</v>
       </c>
       <c r="N5" s="6">
-        <v>10.228565515894701</v>
+        <v>1.3281045709435799</v>
       </c>
       <c r="O5" s="6">
-        <v>3.2345943807963601E-2</v>
+        <v>2.85985170904695</v>
       </c>
       <c r="P5" s="6">
-        <v>26.949882574614101</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>11.169998294241999</v>
-      </c>
-      <c r="R5" s="6">
-        <v>6.5358745123857398</v>
-      </c>
-      <c r="S5" s="6">
-        <v>1.3281045709435799</v>
-      </c>
-      <c r="T5" s="6">
-        <v>2.85985170904695</v>
-      </c>
-      <c r="U5" s="6">
-        <v>0.33985350292187599</v>
-      </c>
-      <c r="V5" s="6">
         <v>15.785966644590999</v>
       </c>
-      <c r="W5" s="6">
-        <v>1.6284915</v>
-      </c>
-      <c r="X5" s="6">
-        <v>25.7073125</v>
-      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>95</v>
       </c>
@@ -6457,73 +6313,49 @@
         <v>1864</v>
       </c>
       <c r="C6" s="4">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4">
-        <v>18</v>
-      </c>
-      <c r="E6" s="4">
         <v>1.0033955999999999</v>
       </c>
+      <c r="E6" s="5">
+        <v>13.298926571882401</v>
+      </c>
       <c r="F6" s="5">
-        <v>13.298926571882401</v>
+        <v>7.7381424731182804</v>
       </c>
       <c r="G6" s="5">
-        <v>7.7381424731182804</v>
+        <v>5.7078853046594998E-2</v>
       </c>
       <c r="H6" s="5">
-        <v>18.108006720430101</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0.58490783410138203</v>
-      </c>
-      <c r="J6" s="5">
-        <v>5.7078853046594998E-2</v>
-      </c>
-      <c r="K6" s="5">
         <v>6</v>
       </c>
+      <c r="I6" s="6">
+        <v>25.195309999999999</v>
+      </c>
+      <c r="J6" s="6">
+        <v>3.4180000000000001</v>
+      </c>
+      <c r="K6" s="6">
+        <v>15.4314263946123</v>
+      </c>
       <c r="L6" s="6">
-        <v>25.195309999999999</v>
+        <v>14.490881088837799</v>
       </c>
       <c r="M6" s="6">
-        <v>3.4180000000000001</v>
+        <v>9.2482468001127796</v>
       </c>
       <c r="N6" s="6">
-        <v>15.4314263946123</v>
+        <v>1.2977686593651101</v>
       </c>
       <c r="O6" s="6">
-        <v>3.4146711803529198E-2</v>
+        <v>4.3765418342962601</v>
       </c>
       <c r="P6" s="6">
-        <v>34.858057843551698</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>14.490881088837799</v>
-      </c>
-      <c r="R6" s="6">
-        <v>9.2482468001127796</v>
-      </c>
-      <c r="S6" s="6">
-        <v>1.2977686593651101</v>
-      </c>
-      <c r="T6" s="6">
-        <v>4.3765418342962601</v>
-      </c>
-      <c r="U6" s="6">
-        <v>0.83199038230143296</v>
-      </c>
-      <c r="V6" s="6">
         <v>15.392849340909899</v>
       </c>
-      <c r="W6" s="6">
-        <v>1.9454849999999999</v>
-      </c>
-      <c r="X6" s="6">
-        <v>29.946557500000001</v>
-      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>96</v>
       </c>
@@ -6534,70 +6366,46 @@
         <v>45</v>
       </c>
       <c r="D7" s="4">
-        <v>45</v>
-      </c>
-      <c r="E7" s="4">
         <v>0.55795289999999997</v>
       </c>
+      <c r="E7" s="5">
+        <v>13.090148588847599</v>
+      </c>
       <c r="F7" s="5">
-        <v>13.090148588847599</v>
+        <v>7.4175060483871</v>
       </c>
       <c r="G7" s="5">
-        <v>7.4175060483871</v>
+        <v>2.7150537634408601E-2</v>
       </c>
       <c r="H7" s="5">
-        <v>18.005200268817202</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0.73591909882232498</v>
-      </c>
-      <c r="J7" s="5">
-        <v>2.7150537634408601E-2</v>
-      </c>
-      <c r="K7" s="5">
         <v>9</v>
       </c>
+      <c r="I7" s="6">
+        <v>17.8125</v>
+      </c>
+      <c r="J7" s="6">
+        <v>3.9020000000000001</v>
+      </c>
+      <c r="K7" s="6">
+        <v>40.516339058225299</v>
+      </c>
       <c r="L7" s="6">
-        <v>17.8125</v>
+        <v>12.4485345301433</v>
       </c>
       <c r="M7" s="6">
-        <v>3.9020000000000001</v>
+        <v>7.2677376957122402</v>
       </c>
       <c r="N7" s="6">
-        <v>40.516339058225299</v>
+        <v>7.1774996774446196</v>
       </c>
       <c r="O7" s="6">
-        <v>7.2301790310405706E-2</v>
+        <v>3.13022821769388</v>
       </c>
       <c r="P7" s="6">
-        <v>16.9154914983819</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>12.4485345301433</v>
-      </c>
-      <c r="R7" s="6">
-        <v>7.2677376957122402</v>
-      </c>
-      <c r="S7" s="6">
-        <v>7.1774996774446196</v>
-      </c>
-      <c r="T7" s="6">
-        <v>3.13022821769388</v>
-      </c>
-      <c r="U7" s="6">
-        <v>0.32847368401358901</v>
-      </c>
-      <c r="V7" s="6">
         <v>12.501842386327301</v>
       </c>
-      <c r="W7" s="6">
-        <v>1.1755135000000001</v>
-      </c>
-      <c r="X7" s="6">
-        <v>14.6960845</v>
-      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>97</v>
       </c>
@@ -6605,73 +6413,49 @@
         <v>1620</v>
       </c>
       <c r="C8" s="4">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="D8" s="4">
-        <v>32</v>
-      </c>
-      <c r="E8" s="4">
         <v>1.0013231</v>
       </c>
+      <c r="E8" s="5">
+        <v>14.2717800053665</v>
+      </c>
       <c r="F8" s="5">
-        <v>14.2717800053665</v>
+        <v>8.7197311827956998</v>
       </c>
       <c r="G8" s="5">
-        <v>8.7197311827956998</v>
+        <v>2.4462365591397899E-2</v>
       </c>
       <c r="H8" s="5">
-        <v>19.1702728494624</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0.58058115719406</v>
-      </c>
-      <c r="J8" s="5">
-        <v>2.4462365591397899E-2</v>
-      </c>
-      <c r="K8" s="5">
         <v>2</v>
       </c>
+      <c r="I8" s="6">
+        <v>26.101559999999999</v>
+      </c>
+      <c r="J8" s="6">
+        <v>3.6269999999999998</v>
+      </c>
+      <c r="K8" s="6">
+        <v>59.557513163232599</v>
+      </c>
       <c r="L8" s="6">
-        <v>26.101559999999999</v>
+        <v>16.746581832331898</v>
       </c>
       <c r="M8" s="6">
-        <v>3.6269999999999998</v>
+        <v>8.5452479540203097</v>
       </c>
       <c r="N8" s="6">
-        <v>59.557513163232599</v>
+        <v>2.0541757028468002</v>
       </c>
       <c r="O8" s="6">
-        <v>3.2727728428586199E-2</v>
+        <v>2.6019260730085998</v>
       </c>
       <c r="P8" s="6">
-        <v>35.437034552062997</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>16.746581832331898</v>
-      </c>
-      <c r="R8" s="6">
-        <v>8.5452479540203097</v>
-      </c>
-      <c r="S8" s="6">
-        <v>2.0541757028468002</v>
-      </c>
-      <c r="T8" s="6">
-        <v>2.6019260730085998</v>
-      </c>
-      <c r="U8" s="6">
-        <v>0.51439292498537303</v>
-      </c>
-      <c r="V8" s="6">
         <v>14.444231499599599</v>
       </c>
-      <c r="W8" s="6">
-        <v>0.96895200000000004</v>
-      </c>
-      <c r="X8" s="6">
-        <v>13.995767000000001</v>
-      </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>98</v>
       </c>
@@ -6679,73 +6463,49 @@
         <v>1625</v>
       </c>
       <c r="C9" s="4">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="D9" s="4">
-        <v>31</v>
-      </c>
-      <c r="E9" s="4">
         <v>0.96260029999999996</v>
       </c>
+      <c r="E9" s="5">
+        <v>14.352429134466901</v>
+      </c>
       <c r="F9" s="5">
-        <v>14.352429134466901</v>
+        <v>8.7299038978494607</v>
       </c>
       <c r="G9" s="5">
-        <v>8.7299038978494607</v>
+        <v>3.5394265232974897E-2</v>
       </c>
       <c r="H9" s="5">
-        <v>19.4740215053763</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0.53560547875064002</v>
-      </c>
-      <c r="J9" s="5">
-        <v>3.5394265232974897E-2</v>
-      </c>
-      <c r="K9" s="5">
         <v>3</v>
       </c>
+      <c r="I9" s="6">
+        <v>34.21875</v>
+      </c>
+      <c r="J9" s="6">
+        <v>3.5049999999999999</v>
+      </c>
+      <c r="K9" s="6">
+        <v>16.510405516382399</v>
+      </c>
       <c r="L9" s="6">
-        <v>34.21875</v>
+        <v>8.0710098367731309</v>
       </c>
       <c r="M9" s="6">
-        <v>3.5049999999999999</v>
+        <v>8.2868857824889304</v>
       </c>
       <c r="N9" s="6">
-        <v>16.510405516382399</v>
+        <v>0.23158191012667501</v>
       </c>
       <c r="O9" s="6">
-        <v>2.7433743457029001E-2</v>
+        <v>1.24402573848996</v>
       </c>
       <c r="P9" s="6">
-        <v>39.903306611932898</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>8.0710098367731309</v>
-      </c>
-      <c r="R9" s="6">
-        <v>8.2868857824889304</v>
-      </c>
-      <c r="S9" s="6">
-        <v>0.23158191012667501</v>
-      </c>
-      <c r="T9" s="6">
-        <v>1.24402573848996</v>
-      </c>
-      <c r="U9" s="6">
-        <v>0.55674785900834001</v>
-      </c>
-      <c r="V9" s="6">
         <v>20.662495083262801</v>
       </c>
-      <c r="W9" s="6">
-        <v>0.36524899999999999</v>
-      </c>
-      <c r="X9" s="6">
-        <v>7.5469556666666699</v>
-      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>99</v>
       </c>
@@ -6753,73 +6513,49 @@
         <v>1540</v>
       </c>
       <c r="C10" s="4">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="D10" s="4">
-        <v>58</v>
-      </c>
-      <c r="E10" s="4">
         <v>0.363506</v>
       </c>
+      <c r="E10" s="5">
+        <v>14.390622136989199</v>
+      </c>
       <c r="F10" s="5">
-        <v>14.390622136989199</v>
+        <v>8.7862553763440907</v>
       </c>
       <c r="G10" s="5">
-        <v>8.7862553763440907</v>
+        <v>3.2706093189964203E-2</v>
       </c>
       <c r="H10" s="5">
-        <v>19.556301075268799</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0.60985663082437302</v>
-      </c>
-      <c r="J10" s="5">
-        <v>3.2706093189964203E-2</v>
-      </c>
-      <c r="K10" s="5">
         <v>2</v>
       </c>
+      <c r="I10" s="6">
+        <v>19.890619999999998</v>
+      </c>
+      <c r="J10" s="6">
+        <v>3.4510000000000001</v>
+      </c>
+      <c r="K10" s="6">
+        <v>54.310719788011603</v>
+      </c>
       <c r="L10" s="6">
-        <v>19.890619999999998</v>
+        <v>26.6395349460266</v>
       </c>
       <c r="M10" s="6">
-        <v>3.4510000000000001</v>
+        <v>28.297227714771601</v>
       </c>
       <c r="N10" s="6">
-        <v>54.310719788011603</v>
+        <v>4.6346349134705704</v>
       </c>
       <c r="O10" s="6">
-        <v>0.104845785630615</v>
+        <v>10.2538137128233</v>
       </c>
       <c r="P10" s="6">
-        <v>32.511771087935998</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>26.6395349460266</v>
-      </c>
-      <c r="R10" s="6">
-        <v>28.297227714771601</v>
-      </c>
-      <c r="S10" s="6">
-        <v>4.6346349134705704</v>
-      </c>
-      <c r="T10" s="6">
-        <v>10.2538137128233</v>
-      </c>
-      <c r="U10" s="6">
-        <v>1.3261183403497201</v>
-      </c>
-      <c r="V10" s="6">
         <v>18.081914061132501</v>
       </c>
-      <c r="W10" s="6">
-        <v>1.8995945000000001</v>
-      </c>
-      <c r="X10" s="6">
-        <v>34.348304499999998</v>
-      </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>100</v>
       </c>
@@ -6827,73 +6563,49 @@
         <v>1350</v>
       </c>
       <c r="C11" s="4">
-        <v>147</v>
+        <v>24</v>
       </c>
       <c r="D11" s="4">
-        <v>24</v>
-      </c>
-      <c r="E11" s="4">
         <v>1.1131831999999999</v>
       </c>
+      <c r="E11" s="5">
+        <v>15.5822924150297</v>
+      </c>
       <c r="F11" s="5">
-        <v>15.5822924150297</v>
+        <v>10.1727762096774</v>
       </c>
       <c r="G11" s="5">
-        <v>10.1727762096774</v>
+        <v>2.16845878136201E-2</v>
       </c>
       <c r="H11" s="5">
-        <v>20.695881720430101</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0.571883000512033</v>
-      </c>
-      <c r="J11" s="5">
-        <v>2.16845878136201E-2</v>
-      </c>
-      <c r="K11" s="5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>20.308589999999999</v>
+      </c>
+      <c r="J11" s="6">
+        <v>3.52</v>
+      </c>
+      <c r="K11" s="6">
+        <v>7.8873748355647004</v>
       </c>
       <c r="L11" s="6">
-        <v>20.308589999999999</v>
+        <v>11.1951537547623</v>
       </c>
       <c r="M11" s="6">
-        <v>3.52</v>
+        <v>4.2394856079559204</v>
       </c>
       <c r="N11" s="6">
-        <v>7.8873748355647004</v>
+        <v>3.1126630096009702</v>
       </c>
       <c r="O11" s="6">
-        <v>4.7716733687252301E-2</v>
+        <v>1.0757841369232599</v>
       </c>
       <c r="P11" s="6">
-        <v>22.878180922125399</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>11.1951537547623</v>
-      </c>
-      <c r="R11" s="6">
-        <v>4.2394856079559204</v>
-      </c>
-      <c r="S11" s="6">
-        <v>3.1126630096009702</v>
-      </c>
-      <c r="T11" s="6">
-        <v>1.0757841369232599</v>
-      </c>
-      <c r="U11" s="6">
-        <v>0.205411682638415</v>
-      </c>
-      <c r="V11" s="6">
         <v>15.1175137228061</v>
       </c>
-      <c r="W11" s="6">
-        <v>0.91608449999999997</v>
-      </c>
-      <c r="X11" s="6">
-        <v>13.84892</v>
-      </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>101</v>
       </c>
@@ -6901,73 +6613,49 @@
         <v>1417</v>
       </c>
       <c r="C12" s="4">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4">
-        <v>20</v>
-      </c>
-      <c r="E12" s="4">
         <v>0.74938400000000005</v>
       </c>
+      <c r="E12" s="5">
+        <v>15.337547098238501</v>
+      </c>
       <c r="F12" s="5">
-        <v>15.337547098238501</v>
+        <v>9.7752768817204299</v>
       </c>
       <c r="G12" s="5">
-        <v>9.7752768817204299</v>
+        <v>2.16845878136201E-2</v>
       </c>
       <c r="H12" s="5">
-        <v>20.617436827957</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0.56077188940092204</v>
-      </c>
-      <c r="J12" s="5">
-        <v>2.16845878136201E-2</v>
-      </c>
-      <c r="K12" s="5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <v>31.570309999999999</v>
+      </c>
+      <c r="J12" s="6">
+        <v>3.1509999999999998</v>
+      </c>
+      <c r="K12" s="6">
+        <v>7.0330010623762904</v>
       </c>
       <c r="L12" s="6">
-        <v>31.570309999999999</v>
+        <v>7.3390278303369598</v>
       </c>
       <c r="M12" s="6">
-        <v>3.1509999999999998</v>
+        <v>12.271186948557</v>
       </c>
       <c r="N12" s="6">
-        <v>7.0330010623762904</v>
+        <v>0.68597338995866997</v>
       </c>
       <c r="O12" s="6">
-        <v>1.92639724658554E-2</v>
+        <v>1.69049521176596</v>
       </c>
       <c r="P12" s="6">
-        <v>33.677604243110999</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>7.3390278303369598</v>
-      </c>
-      <c r="R12" s="6">
-        <v>12.271186948557</v>
-      </c>
-      <c r="S12" s="6">
-        <v>0.68597338995866997</v>
-      </c>
-      <c r="T12" s="6">
-        <v>1.69049521176596</v>
-      </c>
-      <c r="U12" s="6">
-        <v>0.56123946343326903</v>
-      </c>
-      <c r="V12" s="6">
         <v>33.932250855804902</v>
       </c>
-      <c r="W12" s="6">
-        <v>0.56204399999999999</v>
-      </c>
-      <c r="X12" s="6">
-        <v>19.071418000000001</v>
-      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>102</v>
       </c>
@@ -6975,73 +6663,49 @@
         <v>1345</v>
       </c>
       <c r="C13" s="4">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="D13" s="4">
-        <v>45</v>
-      </c>
-      <c r="E13" s="4">
         <v>0.41903479999999999</v>
       </c>
+      <c r="E13" s="5">
+        <v>15.3266215346582</v>
+      </c>
       <c r="F13" s="5">
-        <v>15.3266215346582</v>
+        <v>9.81458266129032</v>
       </c>
       <c r="G13" s="5">
-        <v>9.81458266129032</v>
+        <v>2.16845878136201E-2</v>
       </c>
       <c r="H13" s="5">
-        <v>20.6970168010753</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0.66061827956989205</v>
-      </c>
-      <c r="J13" s="5">
-        <v>2.16845878136201E-2</v>
-      </c>
-      <c r="K13" s="5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I13" s="6">
+        <v>12.285159999999999</v>
+      </c>
+      <c r="J13" s="6">
+        <v>3.629</v>
+      </c>
+      <c r="K13" s="6">
+        <v>11.5444067339904</v>
       </c>
       <c r="L13" s="6">
-        <v>12.285159999999999</v>
+        <v>9.9681671697868808</v>
       </c>
       <c r="M13" s="6">
-        <v>3.629</v>
+        <v>4.5074453191284096</v>
       </c>
       <c r="N13" s="6">
-        <v>11.5444067339904</v>
+        <v>5.3081505133426203</v>
       </c>
       <c r="O13" s="6">
-        <v>8.2272502727698801E-2</v>
+        <v>1.00528265578318</v>
       </c>
       <c r="P13" s="6">
-        <v>20.184363816977299</v>
-      </c>
-      <c r="Q13" s="6">
-        <v>9.9681671697868808</v>
-      </c>
-      <c r="R13" s="6">
-        <v>4.5074453191284096</v>
-      </c>
-      <c r="S13" s="6">
-        <v>5.3081505133426203</v>
-      </c>
-      <c r="T13" s="6">
-        <v>1.00528265578318</v>
-      </c>
-      <c r="U13" s="6">
-        <v>0.32613640900537599</v>
-      </c>
-      <c r="V13" s="6">
         <v>13.9590283961611</v>
       </c>
-      <c r="W13" s="6">
-        <v>0.85909500000000005</v>
-      </c>
-      <c r="X13" s="6">
-        <v>11.992131499999999</v>
-      </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>103</v>
       </c>
@@ -7049,73 +6713,49 @@
         <v>1140</v>
       </c>
       <c r="C14" s="4">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="D14" s="4">
-        <v>13</v>
-      </c>
-      <c r="E14" s="4">
         <v>0.96474669999999996</v>
       </c>
+      <c r="E14" s="5">
+        <v>16.310321303004802</v>
+      </c>
       <c r="F14" s="5">
-        <v>16.310321303004802</v>
+        <v>11.0789756944444</v>
       </c>
       <c r="G14" s="5">
-        <v>11.0789756944444</v>
+        <v>8.0645161290322596E-3</v>
       </c>
       <c r="H14" s="5">
-        <v>21.272385080645201</v>
-      </c>
-      <c r="I14" s="5">
-        <v>0.57826420890937003</v>
-      </c>
-      <c r="J14" s="5">
-        <v>8.0645161290322596E-3</v>
-      </c>
-      <c r="K14" s="5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <v>28.703119999999998</v>
+      </c>
+      <c r="J14" s="6">
+        <v>3.7280000000000002</v>
+      </c>
+      <c r="K14" s="6">
+        <v>11.7302317979557</v>
       </c>
       <c r="L14" s="6">
-        <v>28.703119999999998</v>
+        <v>13.6212552401616</v>
       </c>
       <c r="M14" s="6">
-        <v>3.7280000000000002</v>
+        <v>4.4750480626728004</v>
       </c>
       <c r="N14" s="6">
-        <v>11.7302317979557</v>
+        <v>1.1371364386041101</v>
       </c>
       <c r="O14" s="6">
-        <v>7.4875163193961994E-2</v>
+        <v>1.06225657971508</v>
       </c>
       <c r="P14" s="6">
-        <v>24.767522438697</v>
-      </c>
-      <c r="Q14" s="6">
-        <v>13.6212552401616</v>
-      </c>
-      <c r="R14" s="6">
-        <v>4.4750480626728004</v>
-      </c>
-      <c r="S14" s="6">
-        <v>1.1371364386041101</v>
-      </c>
-      <c r="T14" s="6">
-        <v>1.06225657971508</v>
-      </c>
-      <c r="U14" s="6">
-        <v>0.24117379217163801</v>
-      </c>
-      <c r="V14" s="6">
         <v>14.452246797041299</v>
       </c>
-      <c r="W14" s="6">
-        <v>0.98393399999999998</v>
-      </c>
-      <c r="X14" s="6">
-        <v>14.220057000000001</v>
-      </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>104</v>
       </c>
@@ -7123,73 +6763,49 @@
         <v>1120</v>
       </c>
       <c r="C15" s="4">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="D15" s="4">
-        <v>25</v>
-      </c>
-      <c r="E15" s="4">
         <v>1.0525372</v>
       </c>
+      <c r="E15" s="5">
+        <v>16.6834210374472</v>
+      </c>
       <c r="F15" s="5">
-        <v>16.6834210374472</v>
+        <v>11.4613622311828</v>
       </c>
       <c r="G15" s="5">
-        <v>11.4613622311828</v>
+        <v>1.34408602150538E-2</v>
       </c>
       <c r="H15" s="5">
-        <v>21.735457661290301</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0.364311315924219</v>
-      </c>
-      <c r="J15" s="5">
-        <v>1.34408602150538E-2</v>
-      </c>
-      <c r="K15" s="5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I15" s="6">
+        <v>28.15625</v>
+      </c>
+      <c r="J15" s="6">
+        <v>3.7440000000000002</v>
+      </c>
+      <c r="K15" s="6">
+        <v>10.0697683721276</v>
       </c>
       <c r="L15" s="6">
-        <v>28.15625</v>
+        <v>14.3175797731837</v>
       </c>
       <c r="M15" s="6">
-        <v>3.7440000000000002</v>
+        <v>5.34815297077746</v>
       </c>
       <c r="N15" s="6">
-        <v>10.0697683721276</v>
+        <v>1.0586694857463199</v>
       </c>
       <c r="O15" s="6">
-        <v>6.3425087366589694E-2</v>
+        <v>0.813455967938854</v>
       </c>
       <c r="P15" s="6">
-        <v>26.798816988847999</v>
-      </c>
-      <c r="Q15" s="6">
-        <v>14.3175797731837</v>
-      </c>
-      <c r="R15" s="6">
-        <v>5.34815297077746</v>
-      </c>
-      <c r="S15" s="6">
-        <v>1.0586694857463199</v>
-      </c>
-      <c r="T15" s="6">
-        <v>0.813455967938854</v>
-      </c>
-      <c r="U15" s="6">
-        <v>0.37035028195828501</v>
-      </c>
-      <c r="V15" s="6">
         <v>15.0845177906158</v>
       </c>
-      <c r="W15" s="6">
-        <v>1.0260324999999999</v>
-      </c>
-      <c r="X15" s="6">
-        <v>15.4772055</v>
-      </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>105</v>
       </c>
@@ -7197,73 +6813,49 @@
         <v>1120</v>
       </c>
       <c r="C16" s="4">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D16" s="4">
-        <v>26</v>
-      </c>
-      <c r="E16" s="4">
         <v>0.67469489999999999</v>
       </c>
+      <c r="E16" s="5">
+        <v>16.658455123059699</v>
+      </c>
       <c r="F16" s="5">
-        <v>16.658455123059699</v>
+        <v>11.293918682795701</v>
       </c>
       <c r="G16" s="5">
-        <v>11.293918682795701</v>
+        <v>1.6129032258064498E-2</v>
       </c>
       <c r="H16" s="5">
-        <v>21.830717069892501</v>
-      </c>
-      <c r="I16" s="5">
-        <v>0.42476318484383002</v>
-      </c>
-      <c r="J16" s="5">
-        <v>1.6129032258064498E-2</v>
-      </c>
-      <c r="K16" s="5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I16" s="6">
+        <v>32.921880000000002</v>
+      </c>
+      <c r="J16" s="6">
+        <v>3.758</v>
+      </c>
+      <c r="K16" s="6">
+        <v>8.0950004725418303</v>
       </c>
       <c r="L16" s="6">
-        <v>32.921880000000002</v>
+        <v>14.5281986351171</v>
       </c>
       <c r="M16" s="6">
-        <v>3.758</v>
+        <v>4.4128310452502504</v>
       </c>
       <c r="N16" s="6">
-        <v>8.0950004725418303</v>
+        <v>0.35397887770195002</v>
       </c>
       <c r="O16" s="6">
-        <v>5.26072308616954E-2</v>
+        <v>0.54577509897230603</v>
       </c>
       <c r="P16" s="6">
-        <v>32.956620001543698</v>
-      </c>
-      <c r="Q16" s="6">
-        <v>14.5281986351171</v>
-      </c>
-      <c r="R16" s="6">
-        <v>4.4128310452502504</v>
-      </c>
-      <c r="S16" s="6">
-        <v>0.35397887770195002</v>
-      </c>
-      <c r="T16" s="6">
-        <v>0.54577509897230603</v>
-      </c>
-      <c r="U16" s="6">
-        <v>0.20666426528061399</v>
-      </c>
-      <c r="V16" s="6">
         <v>15.2735349047305</v>
       </c>
-      <c r="W16" s="6">
-        <v>0.83904100000000004</v>
-      </c>
-      <c r="X16" s="6">
-        <v>12.815122000000001</v>
-      </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>106</v>
       </c>
@@ -7271,73 +6863,49 @@
         <v>860</v>
       </c>
       <c r="C17" s="4">
-        <v>125</v>
+        <v>27</v>
       </c>
       <c r="D17" s="4">
-        <v>27</v>
-      </c>
-      <c r="E17" s="4">
         <v>1.0858352</v>
       </c>
+      <c r="E17" s="5">
+        <v>17.7872970768796</v>
+      </c>
       <c r="F17" s="5">
-        <v>17.7872970768796</v>
+        <v>12.5840577956989</v>
       </c>
       <c r="G17" s="5">
-        <v>12.5840577956989</v>
+        <v>5.3763440860214997E-3</v>
       </c>
       <c r="H17" s="5">
-        <v>23.135297715053799</v>
-      </c>
-      <c r="I17" s="5">
-        <v>0.52569124423963098</v>
-      </c>
-      <c r="J17" s="5">
-        <v>5.3763440860214997E-3</v>
-      </c>
-      <c r="K17" s="5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I17" s="6">
+        <v>22.460940000000001</v>
+      </c>
+      <c r="J17" s="6">
+        <v>3.8159999999999998</v>
+      </c>
+      <c r="K17" s="6">
+        <v>13.6656798217541</v>
       </c>
       <c r="L17" s="6">
-        <v>22.460940000000001</v>
+        <v>11.9602463227596</v>
       </c>
       <c r="M17" s="6">
-        <v>3.8159999999999998</v>
+        <v>5.9490683093856704</v>
       </c>
       <c r="N17" s="6">
-        <v>13.6656798217541</v>
+        <v>3.3479205531613898</v>
       </c>
       <c r="O17" s="6">
-        <v>8.0558915961174801E-2</v>
+        <v>0.85722566497947505</v>
       </c>
       <c r="P17" s="6">
-        <v>24.687717314978599</v>
-      </c>
-      <c r="Q17" s="6">
-        <v>11.9602463227596</v>
-      </c>
-      <c r="R17" s="6">
-        <v>5.9490683093856704</v>
-      </c>
-      <c r="S17" s="6">
-        <v>3.3479205531613898</v>
-      </c>
-      <c r="T17" s="6">
-        <v>0.85722566497947505</v>
-      </c>
-      <c r="U17" s="6">
-        <v>0.22388578180177601</v>
-      </c>
-      <c r="V17" s="6">
         <v>13.640948442708099</v>
       </c>
-      <c r="W17" s="6">
-        <v>0.61098050000000004</v>
-      </c>
-      <c r="X17" s="6">
-        <v>8.3343535000000006</v>
-      </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>107</v>
       </c>
@@ -7345,73 +6913,49 @@
         <v>860</v>
       </c>
       <c r="C18" s="4">
-        <v>155</v>
+        <v>23</v>
       </c>
       <c r="D18" s="4">
-        <v>23</v>
-      </c>
-      <c r="E18" s="4">
         <v>1.1095495</v>
       </c>
+      <c r="E18" s="5">
+        <v>17.650601141617798</v>
+      </c>
       <c r="F18" s="5">
-        <v>17.650601141617798</v>
+        <v>12.470317876344099</v>
       </c>
       <c r="G18" s="5">
-        <v>12.470317876344099</v>
+        <v>5.3763440860214997E-3</v>
       </c>
       <c r="H18" s="5">
-        <v>22.9635383064516</v>
-      </c>
-      <c r="I18" s="5">
-        <v>0.54737583205325102</v>
-      </c>
-      <c r="J18" s="5">
-        <v>5.3763440860214997E-3</v>
-      </c>
-      <c r="K18" s="5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I18" s="6">
+        <v>20.76953</v>
+      </c>
+      <c r="J18" s="6">
+        <v>3.8210000000000002</v>
+      </c>
+      <c r="K18" s="6">
+        <v>7.53657865126854</v>
       </c>
       <c r="L18" s="6">
-        <v>20.76953</v>
+        <v>10.157550723003199</v>
       </c>
       <c r="M18" s="6">
-        <v>3.8210000000000002</v>
+        <v>4.6777231691212702</v>
       </c>
       <c r="N18" s="6">
-        <v>7.53657865126854</v>
+        <v>1.12728558320941</v>
       </c>
       <c r="O18" s="6">
-        <v>6.8793587737153702E-2</v>
+        <v>0.64908690361489896</v>
       </c>
       <c r="P18" s="6">
-        <v>31.9599542603139</v>
-      </c>
-      <c r="Q18" s="6">
-        <v>10.157550723003199</v>
-      </c>
-      <c r="R18" s="6">
-        <v>4.6777231691212702</v>
-      </c>
-      <c r="S18" s="6">
-        <v>1.12728558320941</v>
-      </c>
-      <c r="T18" s="6">
-        <v>0.64908690361489896</v>
-      </c>
-      <c r="U18" s="6">
-        <v>0.18758937220090299</v>
-      </c>
-      <c r="V18" s="6">
         <v>13.1799666378983</v>
       </c>
-      <c r="W18" s="6">
-        <v>0.57760149999999999</v>
-      </c>
-      <c r="X18" s="6">
-        <v>7.6127684999999996</v>
-      </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>108</v>
       </c>
@@ -7419,70 +6963,46 @@
         <v>860</v>
       </c>
       <c r="C19" s="4">
-        <v>105</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4">
-        <v>17</v>
-      </c>
-      <c r="E19" s="4">
         <v>1.0454188</v>
       </c>
+      <c r="E19" s="5">
+        <v>17.707419719662099</v>
+      </c>
       <c r="F19" s="5">
-        <v>17.707419719662099</v>
+        <v>12.419131048387101</v>
       </c>
       <c r="G19" s="5">
-        <v>12.419131048387101</v>
+        <v>2.6881720430107499E-3</v>
       </c>
       <c r="H19" s="5">
-        <v>22.979159274193499</v>
-      </c>
-      <c r="I19" s="5">
-        <v>0.70812852022529404</v>
-      </c>
-      <c r="J19" s="5">
-        <v>2.6881720430107499E-3</v>
-      </c>
-      <c r="K19" s="5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I19" s="6">
+        <v>28.570309999999999</v>
+      </c>
+      <c r="J19" s="6">
+        <v>3.657</v>
+      </c>
+      <c r="K19" s="6">
+        <v>5.2589920423832304</v>
       </c>
       <c r="L19" s="6">
-        <v>28.570309999999999</v>
+        <v>10.396982831155</v>
       </c>
       <c r="M19" s="6">
-        <v>3.657</v>
+        <v>5.1721543669344001</v>
       </c>
       <c r="N19" s="6">
-        <v>5.2589920423832304</v>
+        <v>1.5470265526826199</v>
       </c>
       <c r="O19" s="6">
-        <v>9.5268033294682794E-2</v>
+        <v>0.89453986103757199</v>
       </c>
       <c r="P19" s="6">
-        <v>31.023532681028598</v>
-      </c>
-      <c r="Q19" s="6">
-        <v>10.396982831155</v>
-      </c>
-      <c r="R19" s="6">
-        <v>5.1721543669344001</v>
-      </c>
-      <c r="S19" s="6">
-        <v>1.5470265526826199</v>
-      </c>
-      <c r="T19" s="6">
-        <v>0.89453986103757199</v>
-      </c>
-      <c r="U19" s="6">
-        <v>0.278298814869188</v>
-      </c>
-      <c r="V19" s="6">
         <v>13.548438916884599</v>
-      </c>
-      <c r="W19" s="6">
-        <v>0.70467100000000005</v>
-      </c>
-      <c r="X19" s="6">
-        <v>9.5471920000000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>